<commit_message>
finished SetCellValue double and format
</commit_message>
<xml_diff>
--- a/2-Tests/OpenExcelSdk.Tests/10-Files/SetCellValueAndFormat.xlsx
+++ b/2-Tests/OpenExcelSdk.Tests/10-Files/SetCellValueAndFormat.xlsx
@@ -57,7 +57,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -122,7 +122,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,9 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Improve error message in exception
</commit_message>
<xml_diff>
--- a/2-Tests/OpenExcelSdk.Tests/10-Files/SetCellValueAndFormat.xlsx
+++ b/2-Tests/OpenExcelSdk.Tests/10-Files/SetCellValueAndFormat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/10-Pierlam/OpenExcelSdk/Dev/OpenExcelSdk/2-Tests/OpenExcelSdk.Tests/10-Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6E8626F-0C41-4212-9C05-56F2D3266C5F}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16EF60A9-07BE-4F2E-B57C-237A027B1304}"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="2835" windowWidth="16260" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="3030" windowWidth="16155" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -115,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -123,6 +124,7 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +462,7 @@
       <c r="B4" s="6">
         <v>120.5</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>357.2</v>
       </c>
     </row>

</xml_diff>